<commit_message>
In receipt vouchers upload excel schema all fields relating to entry upload should be created.
</commit_message>
<xml_diff>
--- a/IBS/wwwroot/ReadWriteData/SampleFiles/ReceiptVoucher.xlsx
+++ b/IBS/wwwroot/ReadWriteData/SampleFiles/ReceiptVoucher.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Vishal\IBS\IBS\wwwroot\ReadWriteData\SampleFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\IBSRepo\IBS\wwwroot\ReadWriteData\SampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Cheque No</t>
   </si>
@@ -33,6 +33,54 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>Bank/Cash</t>
+  </si>
+  <si>
+    <t>BPO</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Case No</t>
+  </si>
+  <si>
+    <t>Narration</t>
+  </si>
+  <si>
+    <t>ABHYUDAYA CO-OP BANK LTD</t>
+  </si>
+  <si>
+    <t>18669 - ADITYA HIGH VACCUM PVT LTD/PLOT NO 218, 219 PHASE 1 GIDC INDL ESTATE KATHWADA /AHMEDABAD /AHVPL</t>
+  </si>
+  <si>
+    <t>Customer's Advances:2709</t>
+  </si>
+  <si>
+    <t>N24030082</t>
+  </si>
+  <si>
+    <t>Been</t>
+  </si>
+  <si>
+    <t>18670 - ADITYA HIGH VACCUM PVT LTD/PLOT NO 218, 219 PHASE 1 GIDC INDL ESTATE KATHWADA /AHMEDABAD /AHVPL</t>
+  </si>
+  <si>
+    <t>N24030083</t>
+  </si>
+  <si>
+    <t>18671 - ADITYA HIGH VACCUM PVT LTD/PLOT NO 218, 219 PHASE 1 GIDC INDL ESTATE KATHWADA /AHMEDABAD /AHVPL</t>
+  </si>
+  <si>
+    <t>N24030084</t>
+  </si>
+  <si>
+    <t>Fee Receivable Foreign Rly:2202</t>
+  </si>
+  <si>
+    <t>Fee Receivable State Govt.:2205</t>
   </si>
 </sst>
 </file>
@@ -42,7 +90,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,6 +105,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Poppins"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,13 +147,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,20 +435,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="113" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -404,8 +461,23 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="4">
         <v>123</v>
       </c>
@@ -415,8 +487,23 @@
       <c r="C2" s="4">
         <v>100</v>
       </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="4">
         <v>345</v>
       </c>
@@ -426,8 +513,23 @@
       <c r="C3" s="4">
         <v>200</v>
       </c>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="4">
         <v>654</v>
       </c>
@@ -436,6 +538,21 @@
       </c>
       <c r="C4" s="4">
         <v>300</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>